<commit_message>
hotfix(Lỗi API PMIS): đổi sang thư viện restSharp call api Pmis
</commit_message>
<xml_diff>
--- a/ECP_V2.WebApplication/Content/Dvibc-LLV.Tuan_13-11-2024 16_40_32.xlsx
+++ b/ECP_V2.WebApplication/Content/Dvibc-LLV.Tuan_13-11-2024 16_40_32.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhvt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973133D6-6CF1-400D-9D61-B500E492609D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193706C9-BCB2-4E84-88BC-BC8B6F8C9F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2730" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="72">
   <si>
     <t>CỘNG HOÀ XÃ HỘI CHỦ NGHĨA VIỆT NAM</t>
   </si>
@@ -172,9 +172,6 @@
     <t xml:space="preserve"> - Lưu: VT, KH-KT-AT.</t>
   </si>
   <si>
-    <t>Bùi Xuân Hưng TP Kỹ thuật - 0966353888</t>
-  </si>
-  <si>
     <t>Đào Thành Công - 0372752001</t>
   </si>
   <si>
@@ -196,46 +193,49 @@
     <t>Từ ngày 09/12/2024 đến ngày 15/12/2024</t>
   </si>
   <si>
-    <t>Thứ 4, ngày 01/01/2025</t>
-  </si>
-  <si>
-    <t>Thứ 5, ngày 02/01/2025</t>
-  </si>
-  <si>
-    <t>Thứ 6, ngày 03/01/2025</t>
-  </si>
-  <si>
-    <t>Thứ 7, ngày 04/01/2025</t>
-  </si>
-  <si>
-    <t>Chủ nhật, ngày 05/01/2025</t>
-  </si>
-  <si>
-    <t>Công việc 1</t>
-  </si>
-  <si>
-    <t>Công việc 2</t>
-  </si>
-  <si>
-    <t>Công việc 3</t>
-  </si>
-  <si>
-    <t>Thay công tơ định kỳ 1 pha 4</t>
-  </si>
-  <si>
-    <t>Thay công tơ định kỳ 1 pha 5</t>
-  </si>
-  <si>
-    <t>Thay công tơ định kỳ 1 pha 6</t>
-  </si>
-  <si>
-    <t>Thay công tơ định kỳ 1 pha 7</t>
-  </si>
-  <si>
-    <t>Thứ 2, ngày 30/12/2024</t>
-  </si>
-  <si>
-    <t>Thứ 3, ngày 31/12/2024</t>
+    <t xml:space="preserve">Hình thức kiểm tra hiện trường	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đại diện Đoàn KT hiện trường	</t>
+  </si>
+  <si>
+    <t>Bùi Duy Đức-PGĐ ĐL - 0963556777</t>
+  </si>
+  <si>
+    <t>Công tác đầu giờ</t>
+  </si>
+  <si>
+    <t>công việc 1</t>
+  </si>
+  <si>
+    <t>công việc 2</t>
+  </si>
+  <si>
+    <t>công việc 3</t>
+  </si>
+  <si>
+    <t>công việc 4</t>
+  </si>
+  <si>
+    <t>công việc 5</t>
+  </si>
+  <si>
+    <t>công việc 12</t>
+  </si>
+  <si>
+    <t>Thứ 2, ngày 17/03/2025</t>
+  </si>
+  <si>
+    <t>Thứ 3, ngày 18/03/2025</t>
+  </si>
+  <si>
+    <t>Thứ 4, ngày 19/03/2025</t>
+  </si>
+  <si>
+    <t>Thứ 5, ngày 20/03/2025</t>
+  </si>
+  <si>
+    <t>Thứ 6, ngày 21/03/2025</t>
   </si>
 </sst>
 </file>
@@ -254,58 +254,70 @@
       <b/>
       <sz val="13"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="13"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="13"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="13"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -316,7 +328,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -339,48 +351,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -397,16 +372,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -415,18 +393,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -765,10 +731,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -781,132 +747,133 @@
     <col min="7" max="11" width="17.625" customWidth="1" collapsed="1"/>
     <col min="12" max="15" width="11.75" customWidth="1" collapsed="1"/>
     <col min="16" max="17" width="17.625" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="27.25" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="17.625" customWidth="1"/>
+    <col min="20" max="21" width="27.25" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="G1" s="8" t="s">
+    <row r="1" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="G1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="R1" s="1" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="T1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="G2" s="8" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="G2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="R2" s="1" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="T2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="R3" s="1" t="s">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="T3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="G4" s="11" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="G4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="R4" s="1" t="s">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="T4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="R5" s="1" t="s">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="T5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="R6" s="1" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="T6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="R7" s="1" t="s">
+    <row r="7" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="T7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="R8" s="1" t="s">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="T8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -959,22 +926,28 @@
         <v>32</v>
       </c>
       <c r="R9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="T9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S9" s="2" t="s">
+      <c r="U9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="V9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="W9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="V9" s="2" t="s">
+      <c r="X9" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -1026,25 +999,27 @@
       <c r="Q10" s="3">
         <v>18</v>
       </c>
-      <c r="R10" s="3">
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3">
         <v>19</v>
       </c>
-      <c r="S10" s="3">
+      <c r="U10" s="3">
         <v>20</v>
       </c>
-      <c r="T10" s="3">
+      <c r="V10" s="3">
         <v>21</v>
       </c>
-      <c r="U10" s="3">
+      <c r="W10" s="3">
         <v>22</v>
       </c>
-      <c r="V10" s="3">
+      <c r="X10" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1067,16 +1042,18 @@
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
-    </row>
-    <row r="12" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+    </row>
+    <row r="12" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>38</v>
@@ -1085,22 +1062,22 @@
         <v>39</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="K12" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>5</v>
@@ -1115,52 +1092,96 @@
         <v>14</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
-    </row>
-    <row r="13" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="7"/>
-    </row>
-    <row r="14" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+    </row>
+    <row r="13" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>2</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+    </row>
+    <row r="14" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>38</v>
@@ -1169,22 +1190,22 @@
         <v>39</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="4" t="s">
+      <c r="J14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>5</v>
@@ -1199,52 +1220,60 @@
         <v>14</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
-    </row>
-    <row r="15" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
-      <c r="V15" s="7"/>
-    </row>
-    <row r="16" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+    </row>
+    <row r="15" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+    </row>
+    <row r="16" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>38</v>
@@ -1253,22 +1282,22 @@
         <v>39</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="4" t="s">
+      <c r="J16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>5</v>
@@ -1283,52 +1312,60 @@
         <v>14</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
-    </row>
-    <row r="17" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
-      <c r="U17" s="6"/>
-      <c r="V17" s="7"/>
-    </row>
-    <row r="18" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+    </row>
+    <row r="17" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+    </row>
+    <row r="18" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>38</v>
@@ -1337,22 +1374,22 @@
         <v>39</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="H18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I18" s="4" t="s">
+      <c r="J18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="K18" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>5</v>
@@ -1367,52 +1404,60 @@
         <v>14</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
-    </row>
-    <row r="19" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="7"/>
-    </row>
-    <row r="20" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+    </row>
+    <row r="19" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+    </row>
+    <row r="20" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>38</v>
@@ -1421,22 +1466,22 @@
         <v>39</v>
       </c>
       <c r="F20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="H20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I20" s="4" t="s">
+      <c r="J20" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="K20" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>5</v>
@@ -1451,261 +1496,242 @@
         <v>14</v>
       </c>
       <c r="P20" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
-    </row>
-    <row r="21" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="7"/>
-    </row>
-    <row r="22" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
-        <v>1</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="O22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P22" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q22" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+    </row>
+    <row r="21" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+    </row>
+    <row r="22" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
-    </row>
-    <row r="23" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="7"/>
-    </row>
-    <row r="24" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
-        <v>1</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="O24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q24" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+    </row>
+    <row r="23" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+    </row>
+    <row r="24" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
-    </row>
-    <row r="26" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+    </row>
+    <row r="25" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+    </row>
+    <row r="26" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+    </row>
+    <row r="28" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="E26" s="15" t="s">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="E28" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="15" t="s">
+      <c r="F28" s="7"/>
+      <c r="G28" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="15" t="s">
+      <c r="H28" s="7"/>
+      <c r="I28" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="I27" s="15" t="s">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="I29" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="J27" s="9"/>
-    </row>
-    <row r="28" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-    </row>
-    <row r="29" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-    </row>
-    <row r="30" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31" spans="1:22" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A19:V19"/>
-    <mergeCell ref="A17:V17"/>
-    <mergeCell ref="A15:V15"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A21:V21"/>
-    <mergeCell ref="A23:V23"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="A13:V13"/>
+    <mergeCell ref="A15:X15"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="A2:D2"/>
@@ -1717,7 +1743,22 @@
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="A7:J7"/>
     <mergeCell ref="A8:J8"/>
-    <mergeCell ref="A11:V11"/>
+    <mergeCell ref="A11:X11"/>
+    <mergeCell ref="A21:X21"/>
+    <mergeCell ref="A19:X19"/>
+    <mergeCell ref="A17:X17"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A23:X23"/>
+    <mergeCell ref="A25:X25"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape"/>

</xml_diff>